<commit_message>
add get_all_trips method to Flask.
dynamically loads 'trips offered.xlsx'
</commit_message>
<xml_diff>
--- a/mo-service-providers/flask_v1/PROVIDER_DATA/trips offered.xlsx
+++ b/mo-service-providers/flask_v1/PROVIDER_DATA/trips offered.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="17">
   <si>
     <t xml:space="preserve">tripID</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t xml:space="preserve">2018-07-21T145000Z+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-21T185000Z+01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018-07-21T195000Z+01</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -81,6 +87,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -102,6 +109,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -175,16 +183,16 @@
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="15.1377551020408"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6224489795918"/>
-    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="15.1377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="12.9132653061225"/>
+    <col collapsed="false" hidden="false" max="6" min="1" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="27.1326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.2755102040816"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="12.6887755102041"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -243,7 +251,10 @@
         <v>12</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -270,7 +281,10 @@
         <v>12</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I3" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -297,7 +311,10 @@
         <v>12</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I4" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -324,7 +341,10 @@
         <v>12</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I5" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,7 +371,10 @@
         <v>12</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,7 +401,10 @@
         <v>12</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -405,7 +431,10 @@
         <v>12</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -432,7 +461,10 @@
         <v>12</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I9" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -459,7 +491,10 @@
         <v>12</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I10" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -486,7 +521,10 @@
         <v>12</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I11" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -513,7 +551,10 @@
         <v>12</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I12" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -540,7 +581,10 @@
         <v>12</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I13" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -567,7 +611,10 @@
         <v>12</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I14" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -594,7 +641,10 @@
         <v>12</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I15" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -621,7 +671,10 @@
         <v>12</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I16" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -648,7 +701,10 @@
         <v>12</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -675,7 +731,10 @@
         <v>12</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
+      </c>
+      <c r="I18" s="0" t="n">
+        <v>4</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -702,22 +761,13 @@
         <v>12</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>12</v>
+        <v>14</v>
+      </c>
+      <c r="I19" s="0" t="n">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B:B">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="min" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max" val="0"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FF00CC00"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -741,7 +791,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -749,13 +799,13 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -776,9 +826,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="20.2857142857143"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="20.0051020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -786,7 +836,7 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -808,7 +858,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>